<commit_message>
modelo com as equações originais
</commit_message>
<xml_diff>
--- a/DATA/ieee-33.xlsx
+++ b/DATA/ieee-33.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Branch_data" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Branch_loads" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="DLIN" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="DBAR" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="network" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -22,7 +22,235 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="123">
+  <si>
+    <t xml:space="preserve">Linha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R[ohm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X[ohm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bsh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0922</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0477</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.4930</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.2511</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3660</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1864</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3811</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1941</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8190</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1872</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.6188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.7114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2351</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1966</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3744</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4680</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1550</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5416</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7129</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5910</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5260</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7463</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.7210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7320</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5740</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1640</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1565</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3554</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.4095</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.4784</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7089</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9373</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.4512</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3083</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7091</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8960</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.2030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.2842</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1447</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0590</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9337</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.2585</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9744</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9630</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3619</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3410</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Localizacao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P[kw]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q[kvar]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P_Gen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q_Gen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
   <si>
     <t xml:space="preserve">Branch</t>
   </si>
@@ -39,238 +267,40 @@
     <t xml:space="preserve">X</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0922</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0477</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.4930</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.2511</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3660</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1864</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3811</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1941</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8190</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1872</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.6188</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.7114</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2351</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.0300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7400</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.0400</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1966</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0650</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3744</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1238</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.4680</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1550</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.5416</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7129</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.5910</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.5260</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7463</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.5450</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.2890</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.7210</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7320</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.5740</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1640</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1565</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.5042</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.3554</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.4095</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.4784</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7089</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.9373</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.4512</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3083</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8980</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7091</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8960</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.2030</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1034</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.2842</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1447</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.0590</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.9337</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8042</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.7006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.5075</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.2585</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.9744</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.9630</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3105</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3619</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.3410</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.5302</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bus_Location</t>
-  </si>
-  <si>
     <t xml:space="preserve">P</t>
   </si>
   <si>
     <t xml:space="preserve">Q</t>
   </si>
   <si>
-    <t xml:space="preserve">P_Gen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q_Gen</t>
+    <t xml:space="preserve">Cable_Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type_Gen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bus1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bus2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LX95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External Supplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bus3</t>
   </si>
   <si>
     <t xml:space="preserve">NaN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cable_Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type_Gen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bus1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bus2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LX95</t>
-  </si>
-  <si>
-    <t xml:space="preserve">External Supplier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bus3</t>
   </si>
   <si>
     <t xml:space="preserve">bus4</t>
@@ -524,7 +554,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -547,6 +577,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -687,10 +721,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N21" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -711,6 +745,9 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
@@ -723,10 +760,13 @@
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -740,10 +780,13 @@
         <v>3</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -757,10 +800,13 @@
         <v>4</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -774,10 +820,13 @@
         <v>5</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -791,10 +840,13 @@
         <v>6</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -808,10 +860,13 @@
         <v>7</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -825,10 +880,13 @@
         <v>8</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -842,10 +900,13 @@
         <v>9</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -859,10 +920,13 @@
         <v>10</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>20</v>
+      <c r="F10" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -876,10 +940,13 @@
         <v>11</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -893,10 +960,13 @@
         <v>12</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -910,10 +980,13 @@
         <v>13</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -927,10 +1000,13 @@
         <v>14</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -944,10 +1020,13 @@
         <v>15</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -961,10 +1040,13 @@
         <v>16</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -978,10 +1060,13 @@
         <v>17</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -995,10 +1080,13 @@
         <v>18</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1012,10 +1100,13 @@
         <v>19</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1029,10 +1120,13 @@
         <v>20</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1046,10 +1140,13 @@
         <v>21</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1063,10 +1160,13 @@
         <v>22</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1080,10 +1180,13 @@
         <v>23</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1097,10 +1200,13 @@
         <v>24</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1114,10 +1220,13 @@
         <v>25</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1131,10 +1240,13 @@
         <v>26</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1148,10 +1260,13 @@
         <v>27</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1165,10 +1280,13 @@
         <v>28</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1182,10 +1300,13 @@
         <v>29</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1199,10 +1320,13 @@
         <v>30</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1216,10 +1340,13 @@
         <v>31</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1233,10 +1360,13 @@
         <v>32</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1250,10 +1380,13 @@
         <v>33</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1274,8 +1407,8 @@
   </sheetPr>
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1284,42 +1417,42 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>72</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="n">
+      <c r="B2" s="7" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="7" t="n">
+      <c r="D2" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="6" t="n">
+      <c r="E2" s="7" t="n">
         <v>10000</v>
       </c>
-      <c r="F2" s="6" t="n">
+      <c r="F2" s="7" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1327,640 +1460,640 @@
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="n">
+      <c r="B3" s="9" t="n">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="n">
         <v>100</v>
       </c>
-      <c r="D3" s="9" t="n">
+      <c r="D3" s="10" t="n">
         <v>60</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="7" t="n">
         <v>3</v>
       </c>
       <c r="C4" s="3" t="n">
         <v>90</v>
       </c>
-      <c r="D4" s="7" t="n">
+      <c r="D4" s="8" t="n">
         <v>40</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="n">
+      <c r="B5" s="9" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>120</v>
       </c>
-      <c r="D5" s="9" t="n">
+      <c r="D5" s="10" t="n">
         <v>80</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="n">
+      <c r="B6" s="7" t="n">
         <v>5</v>
       </c>
       <c r="C6" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="D6" s="7" t="n">
+      <c r="D6" s="8" t="n">
         <v>30</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="n">
+      <c r="B7" s="9" t="n">
         <v>6</v>
       </c>
       <c r="C7" s="5" t="n">
         <v>60</v>
       </c>
-      <c r="D7" s="9" t="n">
+      <c r="D7" s="10" t="n">
         <v>20</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="n">
+      <c r="B8" s="7" t="n">
         <v>7</v>
       </c>
       <c r="C8" s="3" t="n">
         <v>200</v>
       </c>
-      <c r="D8" s="7" t="n">
+      <c r="D8" s="8" t="n">
         <v>100</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="n">
+      <c r="B9" s="9" t="n">
         <v>8</v>
       </c>
       <c r="C9" s="5" t="n">
         <v>200</v>
       </c>
-      <c r="D9" s="9" t="n">
+      <c r="D9" s="10" t="n">
         <v>100</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="n">
+      <c r="B10" s="7" t="n">
         <v>9</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="D10" s="7" t="n">
+      <c r="D10" s="8" t="n">
         <v>20</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="n">
+      <c r="B11" s="9" t="n">
         <v>10</v>
       </c>
       <c r="C11" s="5" t="n">
         <v>60</v>
       </c>
-      <c r="D11" s="9" t="n">
+      <c r="D11" s="10" t="n">
         <v>20</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="n">
+      <c r="B12" s="7" t="n">
         <v>11</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>45</v>
       </c>
-      <c r="D12" s="7" t="n">
+      <c r="D12" s="8" t="n">
         <v>30</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="n">
+      <c r="B13" s="9" t="n">
         <v>12</v>
       </c>
       <c r="C13" s="5" t="n">
         <v>60</v>
       </c>
-      <c r="D13" s="9" t="n">
+      <c r="D13" s="10" t="n">
         <v>35</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="6" t="n">
+      <c r="B14" s="7" t="n">
         <v>13</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="D14" s="7" t="n">
+      <c r="D14" s="8" t="n">
         <v>35</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="n">
+      <c r="B15" s="9" t="n">
         <v>14</v>
       </c>
       <c r="C15" s="5" t="n">
         <v>120</v>
       </c>
-      <c r="D15" s="9" t="n">
+      <c r="D15" s="10" t="n">
         <v>80</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="6" t="n">
+      <c r="B16" s="7" t="n">
         <v>15</v>
       </c>
       <c r="C16" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="D16" s="7" t="n">
+      <c r="D16" s="8" t="n">
         <v>10</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="n">
+      <c r="B17" s="9" t="n">
         <v>16</v>
       </c>
       <c r="C17" s="5" t="n">
         <v>60</v>
       </c>
-      <c r="D17" s="9" t="n">
+      <c r="D17" s="10" t="n">
         <v>20</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="6" t="n">
+      <c r="B18" s="7" t="n">
         <v>17</v>
       </c>
       <c r="C18" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="D18" s="7" t="n">
+      <c r="D18" s="8" t="n">
         <v>20</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="8" t="n">
+      <c r="B19" s="9" t="n">
         <v>18</v>
       </c>
       <c r="C19" s="5" t="n">
         <v>90</v>
       </c>
-      <c r="D19" s="9" t="n">
+      <c r="D19" s="10" t="n">
         <v>40</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="6" t="n">
+      <c r="B20" s="7" t="n">
         <v>19</v>
       </c>
       <c r="C20" s="3" t="n">
         <v>90</v>
       </c>
-      <c r="D20" s="7" t="n">
+      <c r="D20" s="8" t="n">
         <v>40</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="8" t="n">
+      <c r="B21" s="9" t="n">
         <v>20</v>
       </c>
       <c r="C21" s="5" t="n">
         <v>90</v>
       </c>
-      <c r="D21" s="9" t="n">
+      <c r="D21" s="10" t="n">
         <v>40</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="6" t="n">
+      <c r="B22" s="7" t="n">
         <v>21</v>
       </c>
       <c r="C22" s="3" t="n">
         <v>90</v>
       </c>
-      <c r="D22" s="7" t="n">
+      <c r="D22" s="8" t="n">
         <v>40</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="8" t="n">
+      <c r="B23" s="9" t="n">
         <v>22</v>
       </c>
       <c r="C23" s="5" t="n">
         <v>90</v>
       </c>
-      <c r="D23" s="9" t="n">
+      <c r="D23" s="10" t="n">
         <v>40</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="6" t="n">
+      <c r="B24" s="7" t="n">
         <v>23</v>
       </c>
       <c r="C24" s="3" t="n">
         <v>90</v>
       </c>
-      <c r="D24" s="7" t="n">
+      <c r="D24" s="8" t="n">
         <v>50</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="8" t="n">
+      <c r="B25" s="9" t="n">
         <v>24</v>
       </c>
       <c r="C25" s="5" t="n">
         <v>420</v>
       </c>
-      <c r="D25" s="9" t="n">
+      <c r="D25" s="10" t="n">
         <v>200</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="6" t="n">
+      <c r="B26" s="7" t="n">
         <v>25</v>
       </c>
       <c r="C26" s="3" t="n">
         <v>420</v>
       </c>
-      <c r="D26" s="7" t="n">
+      <c r="D26" s="8" t="n">
         <v>200</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="8" t="n">
+      <c r="B27" s="9" t="n">
         <v>26</v>
       </c>
       <c r="C27" s="5" t="n">
         <v>60</v>
       </c>
-      <c r="D27" s="9" t="n">
+      <c r="D27" s="10" t="n">
         <v>25</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="6" t="n">
+      <c r="B28" s="7" t="n">
         <v>27</v>
       </c>
       <c r="C28" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="D28" s="7" t="n">
+      <c r="D28" s="8" t="n">
         <v>25</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="8" t="n">
+      <c r="B29" s="9" t="n">
         <v>28</v>
       </c>
       <c r="C29" s="5" t="n">
         <v>60</v>
       </c>
-      <c r="D29" s="9" t="n">
+      <c r="D29" s="10" t="n">
         <v>20</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="6" t="n">
+      <c r="B30" s="7" t="n">
         <v>29</v>
       </c>
       <c r="C30" s="3" t="n">
         <v>120</v>
       </c>
-      <c r="D30" s="7" t="n">
+      <c r="D30" s="8" t="n">
         <v>70</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="8" t="n">
+      <c r="B31" s="9" t="n">
         <v>30</v>
       </c>
       <c r="C31" s="5" t="n">
         <v>200</v>
       </c>
-      <c r="D31" s="9" t="n">
+      <c r="D31" s="10" t="n">
         <v>600</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="6" t="n">
+      <c r="B32" s="7" t="n">
         <v>31</v>
       </c>
       <c r="C32" s="3" t="n">
         <v>150</v>
       </c>
-      <c r="D32" s="7" t="n">
+      <c r="D32" s="8" t="n">
         <v>70</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="8" t="n">
+      <c r="B33" s="9" t="n">
         <v>32</v>
       </c>
       <c r="C33" s="5" t="n">
         <v>210</v>
       </c>
-      <c r="D33" s="9" t="n">
+      <c r="D33" s="10" t="n">
         <v>100</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="6" t="n">
+      <c r="B34" s="7" t="n">
         <v>33</v>
       </c>
-      <c r="C34" s="6" t="n">
+      <c r="C34" s="7" t="n">
         <v>60</v>
       </c>
-      <c r="D34" s="10" t="n">
+      <c r="D34" s="11" t="n">
         <v>40</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2000,7 +2133,7 @@
   <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2012,43 +2145,43 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>77</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>78</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>79</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2056,40 +2189,40 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G2" s="7" t="n">
+      <c r="G2" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="H2" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="I2" s="12" t="n">
+      <c r="H2" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" s="13" t="n">
         <v>0.6</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="K2" s="6" t="n">
+      <c r="J2" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="7" t="n">
         <v>10000</v>
       </c>
-      <c r="L2" s="6" t="n">
+      <c r="L2" s="7" t="n">
         <v>10000</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2097,40 +2230,40 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F3" s="5" t="n">
         <v>100</v>
       </c>
-      <c r="G3" s="9" t="n">
+      <c r="G3" s="10" t="n">
         <v>60</v>
       </c>
-      <c r="H3" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="I3" s="12" t="n">
+      <c r="H3" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" s="13" t="n">
         <v>0.75</v>
       </c>
-      <c r="J3" s="8" t="s">
-        <v>73</v>
+      <c r="J3" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2138,40 +2271,40 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>90</v>
       </c>
-      <c r="G4" s="7" t="n">
+      <c r="G4" s="8" t="n">
         <v>40</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="I4" s="12" t="n">
+      <c r="H4" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I4" s="13" t="n">
         <v>0.8</v>
       </c>
-      <c r="J4" s="8" t="s">
-        <v>73</v>
+      <c r="J4" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2179,40 +2312,40 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F5" s="5" t="n">
         <v>120</v>
       </c>
-      <c r="G5" s="9" t="n">
+      <c r="G5" s="10" t="n">
         <v>80</v>
       </c>
-      <c r="H5" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="I5" s="12" t="n">
+      <c r="H5" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I5" s="13" t="n">
         <v>0.75</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>73</v>
+      <c r="J5" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2220,40 +2353,40 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="G6" s="7" t="n">
+      <c r="G6" s="8" t="n">
         <v>30</v>
       </c>
-      <c r="H6" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="I6" s="12" t="n">
+      <c r="H6" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I6" s="13" t="n">
         <v>0.8</v>
       </c>
-      <c r="J6" s="8" t="s">
-        <v>73</v>
+      <c r="J6" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2261,40 +2394,40 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F7" s="5" t="n">
         <v>60</v>
       </c>
-      <c r="G7" s="9" t="n">
+      <c r="G7" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="H7" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="I7" s="12" t="n">
+      <c r="H7" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" s="13" t="n">
         <v>0.6</v>
       </c>
-      <c r="J7" s="8" t="s">
-        <v>73</v>
+      <c r="J7" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2302,40 +2435,40 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F8" s="3" t="n">
         <v>200</v>
       </c>
-      <c r="G8" s="7" t="n">
+      <c r="G8" s="8" t="n">
         <v>100</v>
       </c>
-      <c r="H8" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="I8" s="12" t="n">
+      <c r="H8" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I8" s="13" t="n">
         <v>0.75</v>
       </c>
-      <c r="J8" s="8" t="s">
-        <v>73</v>
+      <c r="J8" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2343,40 +2476,40 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F9" s="5" t="n">
         <v>200</v>
       </c>
-      <c r="G9" s="9" t="n">
+      <c r="G9" s="10" t="n">
         <v>100</v>
       </c>
-      <c r="H9" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="I9" s="12" t="n">
+      <c r="H9" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I9" s="13" t="n">
         <v>0.8</v>
       </c>
-      <c r="J9" s="8" t="s">
-        <v>73</v>
+      <c r="J9" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2384,40 +2517,40 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="F10" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="G10" s="7" t="n">
+      <c r="G10" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="H10" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="I10" s="12" t="n">
+      <c r="H10" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I10" s="13" t="n">
         <v>0.75</v>
       </c>
-      <c r="J10" s="8" t="s">
-        <v>73</v>
+      <c r="J10" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2425,40 +2558,40 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F11" s="5" t="n">
         <v>60</v>
       </c>
-      <c r="G11" s="9" t="n">
+      <c r="G11" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="H11" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="I11" s="12" t="n">
+      <c r="H11" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I11" s="13" t="n">
         <v>0.6</v>
       </c>
-      <c r="J11" s="8" t="s">
-        <v>73</v>
+      <c r="J11" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2466,40 +2599,40 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F12" s="3" t="n">
         <v>45</v>
       </c>
-      <c r="G12" s="7" t="n">
+      <c r="G12" s="8" t="n">
         <v>30</v>
       </c>
-      <c r="H12" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="I12" s="12" t="n">
+      <c r="H12" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I12" s="13" t="n">
         <v>0.8</v>
       </c>
-      <c r="J12" s="8" t="s">
-        <v>73</v>
+      <c r="J12" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2507,40 +2640,40 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F13" s="5" t="n">
         <v>60</v>
       </c>
-      <c r="G13" s="9" t="n">
+      <c r="G13" s="10" t="n">
         <v>35</v>
       </c>
-      <c r="H13" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="I13" s="14" t="n">
+      <c r="H13" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="I13" s="15" t="n">
         <v>0.75</v>
       </c>
-      <c r="J13" s="8" t="s">
-        <v>73</v>
+      <c r="J13" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2548,40 +2681,40 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F14" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="G14" s="7" t="n">
+      <c r="G14" s="8" t="n">
         <v>35</v>
       </c>
-      <c r="H14" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="I14" s="14" t="n">
+      <c r="H14" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="I14" s="15" t="n">
         <v>0.8</v>
       </c>
-      <c r="J14" s="8" t="s">
-        <v>73</v>
+      <c r="J14" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2589,40 +2722,40 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F15" s="5" t="n">
         <v>120</v>
       </c>
-      <c r="G15" s="9" t="n">
+      <c r="G15" s="10" t="n">
         <v>80</v>
       </c>
-      <c r="H15" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="I15" s="14" t="n">
+      <c r="H15" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="I15" s="15" t="n">
         <v>0.6</v>
       </c>
-      <c r="J15" s="8" t="s">
-        <v>73</v>
+      <c r="J15" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2630,40 +2763,40 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F16" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="G16" s="7" t="n">
+      <c r="G16" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="H16" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="I16" s="14" t="n">
+      <c r="H16" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="I16" s="15" t="n">
         <v>0.8</v>
       </c>
-      <c r="J16" s="8" t="s">
-        <v>73</v>
+      <c r="J16" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2671,40 +2804,40 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F17" s="5" t="n">
         <v>60</v>
       </c>
-      <c r="G17" s="9" t="n">
+      <c r="G17" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="H17" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="I17" s="16" t="n">
+      <c r="H17" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I17" s="17" t="n">
         <v>0.75</v>
       </c>
-      <c r="J17" s="8" t="s">
-        <v>73</v>
+      <c r="J17" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2712,40 +2845,40 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F18" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="G18" s="7" t="n">
+      <c r="G18" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="H18" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="I18" s="16" t="n">
+      <c r="H18" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I18" s="17" t="n">
         <v>0.6</v>
       </c>
-      <c r="J18" s="8" t="s">
-        <v>73</v>
+      <c r="J18" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2753,40 +2886,40 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F19" s="5" t="n">
         <v>90</v>
       </c>
-      <c r="G19" s="9" t="n">
+      <c r="G19" s="10" t="n">
         <v>40</v>
       </c>
-      <c r="H19" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="I19" s="16" t="n">
+      <c r="H19" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I19" s="17" t="n">
         <v>0.8</v>
       </c>
-      <c r="J19" s="8" t="s">
-        <v>73</v>
+      <c r="J19" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2794,40 +2927,40 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F20" s="3" t="n">
         <v>90</v>
       </c>
-      <c r="G20" s="7" t="n">
+      <c r="G20" s="8" t="n">
         <v>40</v>
       </c>
-      <c r="H20" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="I20" s="16" t="n">
+      <c r="H20" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I20" s="17" t="n">
         <v>0.75</v>
       </c>
-      <c r="J20" s="8" t="s">
-        <v>73</v>
+      <c r="J20" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2835,40 +2968,40 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F21" s="5" t="n">
         <v>90</v>
       </c>
-      <c r="G21" s="9" t="n">
+      <c r="G21" s="10" t="n">
         <v>40</v>
       </c>
-      <c r="H21" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="I21" s="16" t="n">
+      <c r="H21" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I21" s="17" t="n">
         <v>0.8</v>
       </c>
-      <c r="J21" s="8" t="s">
-        <v>73</v>
+      <c r="J21" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2876,40 +3009,40 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F22" s="3" t="n">
         <v>90</v>
       </c>
-      <c r="G22" s="7" t="n">
+      <c r="G22" s="8" t="n">
         <v>40</v>
       </c>
-      <c r="H22" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="I22" s="16" t="n">
+      <c r="H22" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I22" s="17" t="n">
         <v>0.6</v>
       </c>
-      <c r="J22" s="8" t="s">
-        <v>73</v>
+      <c r="J22" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2917,40 +3050,40 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F23" s="5" t="n">
         <v>90</v>
       </c>
-      <c r="G23" s="9" t="n">
+      <c r="G23" s="10" t="n">
         <v>40</v>
       </c>
-      <c r="H23" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="I23" s="16" t="n">
+      <c r="H23" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I23" s="17" t="n">
         <v>0.75</v>
       </c>
-      <c r="J23" s="8" t="s">
-        <v>73</v>
+      <c r="J23" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2958,40 +3091,40 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F24" s="3" t="n">
         <v>90</v>
       </c>
-      <c r="G24" s="7" t="n">
+      <c r="G24" s="8" t="n">
         <v>50</v>
       </c>
-      <c r="H24" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="I24" s="16" t="n">
+      <c r="H24" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I24" s="17" t="n">
         <v>0.8</v>
       </c>
-      <c r="J24" s="8" t="s">
-        <v>73</v>
+      <c r="J24" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2999,40 +3132,40 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F25" s="5" t="n">
         <v>420</v>
       </c>
-      <c r="G25" s="9" t="n">
+      <c r="G25" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="H25" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="I25" s="16" t="n">
+      <c r="H25" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I25" s="17" t="n">
         <v>0.75</v>
       </c>
-      <c r="J25" s="8" t="s">
-        <v>73</v>
+      <c r="J25" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3040,40 +3173,40 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F26" s="3" t="n">
         <v>420</v>
       </c>
-      <c r="G26" s="7" t="n">
+      <c r="G26" s="8" t="n">
         <v>200</v>
       </c>
-      <c r="H26" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="I26" s="16" t="n">
+      <c r="H26" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I26" s="17" t="n">
         <v>0.6</v>
       </c>
-      <c r="J26" s="8" t="s">
-        <v>73</v>
+      <c r="J26" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3081,40 +3214,40 @@
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F27" s="5" t="n">
         <v>60</v>
       </c>
-      <c r="G27" s="9" t="n">
+      <c r="G27" s="10" t="n">
         <v>25</v>
       </c>
-      <c r="H27" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="I27" s="18" t="n">
+      <c r="H27" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="I27" s="19" t="n">
         <v>0.8</v>
       </c>
-      <c r="J27" s="8" t="s">
-        <v>73</v>
+      <c r="J27" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3122,40 +3255,40 @@
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F28" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="G28" s="7" t="n">
+      <c r="G28" s="8" t="n">
         <v>25</v>
       </c>
-      <c r="H28" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="I28" s="18" t="n">
+      <c r="H28" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="I28" s="19" t="n">
         <v>0.75</v>
       </c>
-      <c r="J28" s="8" t="s">
-        <v>73</v>
+      <c r="J28" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3163,40 +3296,40 @@
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F29" s="5" t="n">
         <v>60</v>
       </c>
-      <c r="G29" s="9" t="n">
+      <c r="G29" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="H29" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="I29" s="18" t="n">
+      <c r="H29" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="I29" s="19" t="n">
         <v>0.6</v>
       </c>
-      <c r="J29" s="8" t="s">
-        <v>73</v>
+      <c r="J29" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3204,40 +3337,40 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F30" s="3" t="n">
         <v>120</v>
       </c>
-      <c r="G30" s="7" t="n">
+      <c r="G30" s="8" t="n">
         <v>70</v>
       </c>
-      <c r="H30" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="I30" s="18" t="n">
+      <c r="H30" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="I30" s="19" t="n">
         <v>0.75</v>
       </c>
-      <c r="J30" s="8" t="s">
-        <v>73</v>
+      <c r="J30" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3245,40 +3378,40 @@
         <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F31" s="5" t="n">
         <v>200</v>
       </c>
-      <c r="G31" s="9" t="n">
+      <c r="G31" s="10" t="n">
         <v>600</v>
       </c>
-      <c r="H31" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="I31" s="18" t="n">
+      <c r="H31" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="I31" s="19" t="n">
         <v>0.6</v>
       </c>
-      <c r="J31" s="8" t="s">
-        <v>73</v>
+      <c r="J31" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3286,40 +3419,40 @@
         <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F32" s="3" t="n">
         <v>150</v>
       </c>
-      <c r="G32" s="7" t="n">
+      <c r="G32" s="8" t="n">
         <v>70</v>
       </c>
-      <c r="H32" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="I32" s="18" t="n">
+      <c r="H32" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="I32" s="19" t="n">
         <v>0.8</v>
       </c>
-      <c r="J32" s="8" t="s">
-        <v>73</v>
+      <c r="J32" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3327,71 +3460,71 @@
         <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F33" s="5" t="n">
         <v>210</v>
       </c>
-      <c r="G33" s="9" t="n">
+      <c r="G33" s="10" t="n">
         <v>100</v>
       </c>
-      <c r="H33" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="I33" s="18" t="n">
+      <c r="H33" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="I33" s="19" t="n">
         <v>0.75</v>
       </c>
-      <c r="J33" s="8" t="s">
-        <v>73</v>
+      <c r="J33" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="21"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="21"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="21"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="21"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>

</xml_diff>